<commit_message>
Updated effort measurements document
</commit_message>
<xml_diff>
--- a/Assignments/RedEyesBlackDragons_Estimated_Effort.xlsx
+++ b/Assignments/RedEyesBlackDragons_Estimated_Effort.xlsx
@@ -177,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -211,13 +211,10 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
       <sz val="10.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -225,20 +222,13 @@
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12.0"/>
       <color rgb="FF800000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -530,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="162">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -558,7 +548,7 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -588,9 +578,6 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -607,9 +594,6 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -631,9 +615,6 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -660,9 +641,6 @@
     <xf borderId="17" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="19" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -681,13 +659,10 @@
     <xf borderId="18" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="18" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="3" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -696,16 +671,19 @@
     <xf borderId="13" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="4" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="17" fillId="4" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="3" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="18" fillId="3" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="18" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -732,10 +710,7 @@
     <xf borderId="21" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="20" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="19" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -744,16 +719,13 @@
     <xf borderId="19" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="22" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="13" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -768,13 +740,10 @@
     <xf borderId="13" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="13" fillId="4" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -789,22 +758,22 @@
     <xf borderId="18" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="20" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="19" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="19" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="19" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="19" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="19" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -816,22 +785,10 @@
     <xf borderId="18" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="18" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="19" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -855,16 +812,13 @@
     <xf borderId="8" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="23" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="5" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="17" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -879,22 +833,19 @@
     <xf borderId="17" fillId="4" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="18" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="18" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="18" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="18" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="5" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="22" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -903,7 +854,7 @@
     <xf borderId="13" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="17" fillId="4" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -912,25 +863,19 @@
     <xf borderId="17" fillId="4" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="4" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="18" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="18" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="18" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -948,16 +893,13 @@
     <xf borderId="8" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="23" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="19" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -975,16 +917,13 @@
     <xf borderId="21" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="21" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="19" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1011,9 +950,6 @@
     <xf borderId="8" fillId="5" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="5" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1029,16 +965,13 @@
     <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="21" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1050,25 +983,25 @@
     <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="17" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="6" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="17" fillId="6" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1432,13 +1365,13 @@
       <c r="O3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="P3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="Q3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="R3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="S3" s="18"/>
@@ -1459,47 +1392,47 @@
       <c r="AH3" s="5"/>
     </row>
     <row r="4" ht="29.25" customHeight="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="23" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="26" t="s">
+      <c r="R4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="S4" s="25"/>
+      <c r="S4" s="24"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -1517,27 +1450,27 @@
       <c r="AH4" s="5"/>
     </row>
     <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="33"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -1555,35 +1488,35 @@
       <c r="AH5" s="5"/>
     </row>
     <row r="6" ht="15.0" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38">
         <f>SUM(F7)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41">
+      <c r="H6" s="37"/>
+      <c r="I6" s="38">
         <f>SUM(H7)</f>
         <v>0</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="42"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
@@ -1601,37 +1534,37 @@
       <c r="AH6" s="4"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="48"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="50">
+      <c r="M7" s="46">
         <v>0.0</v>
       </c>
-      <c r="N7" s="51">
+      <c r="N7" s="47">
         <v>0.0</v>
       </c>
-      <c r="O7" s="52">
+      <c r="O7" s="47">
         <v>0.0</v>
       </c>
-      <c r="P7" s="52">
+      <c r="P7" s="47">
         <v>0.0</v>
       </c>
-      <c r="Q7" s="52">
+      <c r="Q7" s="47">
         <v>0.0</v>
       </c>
-      <c r="R7" s="52">
+      <c r="R7" s="47">
         <v>0.0</v>
       </c>
-      <c r="S7" s="53">
+      <c r="S7" s="48">
         <f t="shared" ref="S7:S14" si="1">SUM(M7:R7)</f>
         <v>0</v>
       </c>
@@ -1652,33 +1585,33 @@
       <c r="AH7" s="4"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41">
+      <c r="C8" s="34"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38">
         <f>SUM(F9:F11)</f>
         <v>5.5</v>
       </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41">
+      <c r="H8" s="37"/>
+      <c r="I8" s="38">
         <f>SUM(H9:H11)</f>
         <v>5.5</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="55">
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1699,45 +1632,47 @@
       <c r="AH8" s="4"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="44" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="43">
         <v>1.5</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="47">
+      <c r="G9" s="44"/>
+      <c r="H9" s="43">
         <v>1.5</v>
       </c>
-      <c r="I9" s="48"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="51">
+      <c r="M9" s="47">
         <v>2.0</v>
       </c>
-      <c r="N9" s="51">
+      <c r="N9" s="47">
         <v>1.0</v>
       </c>
-      <c r="O9" s="50">
+      <c r="O9" s="46">
         <v>1.0</v>
       </c>
-      <c r="P9" s="50">
+      <c r="P9" s="46">
         <v>1.0</v>
       </c>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="58">
+      <c r="Q9" s="47"/>
+      <c r="R9" s="53">
+        <v>1.0</v>
+      </c>
+      <c r="S9" s="54">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -1756,45 +1691,47 @@
       <c r="AH9" s="4"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="44" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="43">
         <v>3.0</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="47">
+      <c r="G10" s="44"/>
+      <c r="H10" s="43">
         <v>3.0</v>
       </c>
-      <c r="I10" s="48"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="51">
+      <c r="M10" s="47">
         <v>2.0</v>
       </c>
-      <c r="N10" s="51">
+      <c r="N10" s="47">
         <v>1.0</v>
       </c>
-      <c r="O10" s="50">
+      <c r="O10" s="46">
         <v>2.0</v>
       </c>
-      <c r="P10" s="50">
+      <c r="P10" s="46">
         <v>2.0</v>
       </c>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="58">
+      <c r="Q10" s="47"/>
+      <c r="R10" s="53">
+        <v>2.0</v>
+      </c>
+      <c r="S10" s="54">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -1813,45 +1750,47 @@
       <c r="AH10" s="4"/>
     </row>
     <row r="11" ht="15.0" customHeight="1">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="44" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="43">
         <v>1.0</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="47">
+      <c r="G11" s="44"/>
+      <c r="H11" s="43">
         <v>1.0</v>
       </c>
-      <c r="I11" s="48"/>
+      <c r="I11" s="44"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="51">
+      <c r="M11" s="47">
         <v>1.0</v>
       </c>
-      <c r="N11" s="51">
+      <c r="N11" s="47">
         <v>2.0</v>
       </c>
-      <c r="O11" s="50">
+      <c r="O11" s="46">
         <v>1.0</v>
       </c>
-      <c r="P11" s="50">
+      <c r="P11" s="46">
         <v>1.0</v>
       </c>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="58">
+      <c r="Q11" s="47"/>
+      <c r="R11" s="53">
+        <v>1.0</v>
+      </c>
+      <c r="S11" s="54">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -1870,33 +1809,33 @@
       <c r="AH11" s="4"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41">
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38">
         <f>SUM(F13:F14)</f>
         <v>3</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41">
+      <c r="H12" s="37"/>
+      <c r="I12" s="38">
         <f>SUM(H13:H14)</f>
         <v>3</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="55">
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1917,45 +1856,47 @@
       <c r="AH12" s="4"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="59" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="45">
         <v>2.0</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="47">
+      <c r="G13" s="44"/>
+      <c r="H13" s="43">
         <v>2.0</v>
       </c>
-      <c r="I13" s="48"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="51">
+      <c r="M13" s="47">
         <v>0.0</v>
       </c>
-      <c r="N13" s="51">
+      <c r="N13" s="47">
         <v>3.0</v>
       </c>
-      <c r="O13" s="50">
+      <c r="O13" s="46">
         <v>2.0</v>
       </c>
-      <c r="P13" s="50">
+      <c r="P13" s="46">
         <v>2.0</v>
       </c>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="58">
+      <c r="Q13" s="47"/>
+      <c r="R13" s="53">
+        <v>2.0</v>
+      </c>
+      <c r="S13" s="54">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
@@ -1974,45 +1915,47 @@
       <c r="AH13" s="4"/>
     </row>
     <row r="14" ht="15.0" customHeight="1">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="44" t="s">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="43">
         <v>1.0</v>
       </c>
-      <c r="G14" s="48"/>
-      <c r="H14" s="47">
+      <c r="G14" s="44"/>
+      <c r="H14" s="43">
         <v>1.0</v>
       </c>
-      <c r="I14" s="48"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="51">
+      <c r="M14" s="47">
         <v>0.5</v>
       </c>
-      <c r="N14" s="51">
+      <c r="N14" s="47">
         <v>3.0</v>
       </c>
-      <c r="O14" s="50">
+      <c r="O14" s="46">
         <v>1.0</v>
       </c>
-      <c r="P14" s="50">
+      <c r="P14" s="46">
         <v>1.0</v>
       </c>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="58">
+      <c r="Q14" s="47"/>
+      <c r="R14" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="S14" s="54">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -2031,27 +1974,27 @@
       <c r="AH14" s="4"/>
     </row>
     <row r="15" ht="15.0" customHeight="1">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="68"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="63"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="70"/>
-      <c r="S15" s="71"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="64"/>
+      <c r="Q15" s="64"/>
+      <c r="R15" s="64"/>
+      <c r="S15" s="65"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
@@ -2069,35 +2012,35 @@
       <c r="AH15" s="4"/>
     </row>
     <row r="16" ht="15.0" customHeight="1">
-      <c r="A16" s="72" t="s">
+      <c r="A16" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="41">
+      <c r="C16" s="68"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="38">
         <f>SUM(F17:F20)</f>
         <v>31</v>
       </c>
-      <c r="H16" s="77"/>
-      <c r="I16" s="41">
+      <c r="H16" s="71"/>
+      <c r="I16" s="38">
         <f>SUM(H17:H20)</f>
         <v>31</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="78"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="79"/>
-      <c r="S16" s="80">
+      <c r="M16" s="72"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="72"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="73">
         <f t="shared" ref="S16:S19" si="2">SUM(M16:R16)</f>
         <v>0</v>
       </c>
@@ -2118,43 +2061,47 @@
       <c r="AH16" s="5"/>
     </row>
     <row r="17" ht="15.0" customHeight="1">
-      <c r="A17" s="72"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="82" t="s">
+      <c r="A17" s="66"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="84" t="s">
+      <c r="E17" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="85">
+      <c r="F17" s="78">
         <v>20.0</v>
       </c>
-      <c r="G17" s="86"/>
-      <c r="H17" s="85">
+      <c r="G17" s="79"/>
+      <c r="H17" s="78">
         <v>20.0</v>
       </c>
-      <c r="I17" s="87"/>
+      <c r="I17" s="80"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="88"/>
-      <c r="N17" s="89">
+      <c r="M17" s="81">
         <v>3.0</v>
       </c>
-      <c r="O17" s="89">
+      <c r="N17" s="82">
         <v>3.0</v>
       </c>
-      <c r="P17" s="89">
+      <c r="O17" s="82">
         <v>3.0</v>
       </c>
-      <c r="Q17" s="88"/>
-      <c r="R17" s="90"/>
-      <c r="S17" s="91">
+      <c r="P17" s="82">
+        <v>3.0</v>
+      </c>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="81">
+        <v>3.0</v>
+      </c>
+      <c r="S17" s="84">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
@@ -2173,43 +2120,47 @@
       <c r="AH17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="72"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="82" t="s">
+      <c r="A18" s="66"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="84" t="s">
+      <c r="E18" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="85">
+      <c r="F18" s="78">
         <v>10.0</v>
       </c>
-      <c r="G18" s="86"/>
-      <c r="H18" s="85">
+      <c r="G18" s="79"/>
+      <c r="H18" s="78">
         <v>10.0</v>
       </c>
-      <c r="I18" s="86"/>
+      <c r="I18" s="79"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="88"/>
-      <c r="N18" s="89">
+      <c r="M18" s="81">
         <v>3.0</v>
       </c>
-      <c r="O18" s="89">
+      <c r="N18" s="82">
         <v>3.0</v>
       </c>
-      <c r="P18" s="89">
+      <c r="O18" s="82">
         <v>3.0</v>
       </c>
-      <c r="Q18" s="88"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="91">
+      <c r="P18" s="82">
+        <v>3.0</v>
+      </c>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="81">
+        <v>3.0</v>
+      </c>
+      <c r="S18" s="84">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
@@ -2228,43 +2179,47 @@
       <c r="AH18" s="4"/>
     </row>
     <row r="19" ht="15.0" customHeight="1">
-      <c r="A19" s="72"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="82" t="s">
+      <c r="A19" s="66"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="E19" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="85">
+      <c r="F19" s="78">
         <v>1.0</v>
       </c>
-      <c r="G19" s="86"/>
-      <c r="H19" s="85">
+      <c r="G19" s="79"/>
+      <c r="H19" s="78">
         <v>1.0</v>
       </c>
-      <c r="I19" s="86"/>
+      <c r="I19" s="79"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="89">
+      <c r="M19" s="81">
         <v>1.0</v>
       </c>
-      <c r="O19" s="89">
+      <c r="N19" s="82">
         <v>1.0</v>
       </c>
-      <c r="P19" s="89">
+      <c r="O19" s="82">
         <v>1.0</v>
       </c>
-      <c r="Q19" s="88"/>
-      <c r="R19" s="90"/>
-      <c r="S19" s="91">
+      <c r="P19" s="82">
+        <v>1.0</v>
+      </c>
+      <c r="Q19" s="83"/>
+      <c r="R19" s="81">
+        <v>1.0</v>
+      </c>
+      <c r="S19" s="84">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
@@ -2283,25 +2238,25 @@
       <c r="AH19" s="4"/>
     </row>
     <row r="20" ht="15.0" customHeight="1">
-      <c r="A20" s="72"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="86"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="79"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="95"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="83"/>
+      <c r="R20" s="83"/>
+      <c r="S20" s="84"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
@@ -2319,33 +2274,33 @@
       <c r="AH20" s="4"/>
     </row>
     <row r="21" ht="15.0" customHeight="1">
-      <c r="A21" s="72"/>
-      <c r="B21" s="96" t="s">
+      <c r="A21" s="66"/>
+      <c r="B21" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="74"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="41">
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="38">
         <f>SUM(F22:F25)</f>
         <v>2.5</v>
       </c>
-      <c r="H21" s="98"/>
-      <c r="I21" s="41">
+      <c r="H21" s="71"/>
+      <c r="I21" s="38">
         <f>SUM(H22:H25)</f>
         <v>2.5</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="97"/>
-      <c r="N21" s="97"/>
-      <c r="O21" s="97"/>
-      <c r="P21" s="97"/>
-      <c r="Q21" s="97"/>
-      <c r="R21" s="97"/>
-      <c r="S21" s="97"/>
+      <c r="M21" s="70"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="70"/>
+      <c r="P21" s="70"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
+      <c r="S21" s="70"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
@@ -2363,41 +2318,45 @@
       <c r="AH21" s="4"/>
     </row>
     <row r="22" ht="15.0" customHeight="1">
-      <c r="A22" s="72"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="82" t="s">
+      <c r="A22" s="66"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="84" t="s">
+      <c r="E22" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="85">
+      <c r="F22" s="78">
         <v>2.5</v>
       </c>
-      <c r="G22" s="86"/>
-      <c r="H22" s="85">
+      <c r="G22" s="79"/>
+      <c r="H22" s="78">
         <v>2.5</v>
       </c>
-      <c r="I22" s="86"/>
+      <c r="I22" s="79"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="89">
+      <c r="M22" s="81">
         <v>0.0</v>
       </c>
-      <c r="O22" s="89">
+      <c r="N22" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="O22" s="82">
         <v>2.5</v>
       </c>
-      <c r="P22" s="89">
+      <c r="P22" s="82">
         <v>0.0</v>
       </c>
-      <c r="Q22" s="88"/>
-      <c r="R22" s="90"/>
-      <c r="S22" s="91">
+      <c r="Q22" s="83"/>
+      <c r="R22" s="81">
+        <v>0.0</v>
+      </c>
+      <c r="S22" s="84">
         <f t="shared" ref="S22:S23" si="3">SUM(M22:R22)</f>
         <v>2.5</v>
       </c>
@@ -2418,35 +2377,39 @@
       <c r="AH22" s="4"/>
     </row>
     <row r="23" ht="15.0" customHeight="1">
-      <c r="A23" s="72"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="82" t="s">
+      <c r="A23" s="66"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="100" t="s">
+      <c r="D23" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="84" t="s">
+      <c r="E23" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="94"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="86"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="79"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="89">
+      <c r="M23" s="81">
         <v>0.0</v>
       </c>
-      <c r="O23" s="88"/>
-      <c r="P23" s="89">
+      <c r="N23" s="82">
         <v>0.0</v>
       </c>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="90"/>
-      <c r="S23" s="91">
+      <c r="O23" s="83"/>
+      <c r="P23" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="81">
+        <v>0.0</v>
+      </c>
+      <c r="S23" s="84">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2467,25 +2430,25 @@
       <c r="AH23" s="4"/>
     </row>
     <row r="24" ht="15.0" customHeight="1">
-      <c r="A24" s="72"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="86"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="79"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="88"/>
-      <c r="P24" s="88"/>
-      <c r="Q24" s="88"/>
-      <c r="R24" s="90"/>
-      <c r="S24" s="95"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="83"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="83"/>
+      <c r="S24" s="84"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
@@ -2503,25 +2466,25 @@
       <c r="AH24" s="4"/>
     </row>
     <row r="25" ht="15.0" customHeight="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="104"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="107"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="107"/>
-      <c r="I25" s="108"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="97"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="109"/>
-      <c r="N25" s="109"/>
-      <c r="O25" s="109"/>
-      <c r="P25" s="109"/>
-      <c r="Q25" s="109"/>
-      <c r="R25" s="110"/>
-      <c r="S25" s="111"/>
+      <c r="M25" s="98"/>
+      <c r="N25" s="98"/>
+      <c r="O25" s="98"/>
+      <c r="P25" s="98"/>
+      <c r="Q25" s="98"/>
+      <c r="R25" s="98"/>
+      <c r="S25" s="99"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
@@ -2539,33 +2502,33 @@
       <c r="AH25" s="4"/>
     </row>
     <row r="26" ht="15.0" customHeight="1">
-      <c r="A26" s="72"/>
-      <c r="B26" s="112" t="s">
+      <c r="A26" s="66"/>
+      <c r="B26" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="113"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="41">
+      <c r="C26" s="101"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="38">
         <f>SUM(F27:F29)</f>
         <v>20</v>
       </c>
-      <c r="H26" s="114"/>
-      <c r="I26" s="41">
+      <c r="H26" s="102"/>
+      <c r="I26" s="38">
         <f>SUM(H27:H29)</f>
         <v>20</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="115">
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="103">
         <f t="shared" ref="S26:S27" si="4">SUM(M26:R26)</f>
         <v>0</v>
       </c>
@@ -2586,43 +2549,47 @@
       <c r="AH26" s="4"/>
     </row>
     <row r="27" ht="15.0" customHeight="1">
-      <c r="A27" s="72"/>
-      <c r="B27" s="99"/>
-      <c r="C27" s="82" t="s">
+      <c r="A27" s="66"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="83" t="s">
+      <c r="D27" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="116" t="s">
+      <c r="E27" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="85">
+      <c r="F27" s="78">
         <v>20.0</v>
       </c>
-      <c r="G27" s="86"/>
-      <c r="H27" s="85">
+      <c r="G27" s="79"/>
+      <c r="H27" s="78">
         <v>20.0</v>
       </c>
-      <c r="I27" s="86"/>
+      <c r="I27" s="79"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="117"/>
-      <c r="N27" s="118">
+      <c r="M27" s="105">
         <v>3.0</v>
       </c>
-      <c r="O27" s="118">
+      <c r="N27" s="106">
         <v>3.0</v>
       </c>
-      <c r="P27" s="118">
+      <c r="O27" s="106">
         <v>3.0</v>
       </c>
-      <c r="Q27" s="117"/>
-      <c r="R27" s="119"/>
-      <c r="S27" s="120">
+      <c r="P27" s="106">
+        <v>3.0</v>
+      </c>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="105">
+        <v>3.0</v>
+      </c>
+      <c r="S27" s="108">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
@@ -2641,25 +2608,25 @@
       <c r="AH27" s="4"/>
     </row>
     <row r="28" ht="15.0" customHeight="1">
-      <c r="A28" s="72"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="93"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="86"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="79"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="117"/>
-      <c r="N28" s="117"/>
-      <c r="O28" s="117"/>
-      <c r="P28" s="117"/>
-      <c r="Q28" s="117"/>
-      <c r="R28" s="119"/>
-      <c r="S28" s="121"/>
+      <c r="M28" s="107"/>
+      <c r="N28" s="107"/>
+      <c r="O28" s="107"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="108"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
@@ -2677,25 +2644,25 @@
       <c r="AH28" s="4"/>
     </row>
     <row r="29" ht="15.0" customHeight="1">
-      <c r="A29" s="72"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="102"/>
-      <c r="F29" s="94"/>
-      <c r="G29" s="86"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="86"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="79"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="117"/>
-      <c r="N29" s="117"/>
-      <c r="O29" s="117"/>
-      <c r="P29" s="117"/>
-      <c r="Q29" s="117"/>
-      <c r="R29" s="119"/>
-      <c r="S29" s="121"/>
+      <c r="M29" s="107"/>
+      <c r="N29" s="107"/>
+      <c r="O29" s="107"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="108"/>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
@@ -2713,35 +2680,35 @@
       <c r="AH29" s="4"/>
     </row>
     <row r="30" ht="15.0" customHeight="1">
-      <c r="A30" s="122" t="s">
+      <c r="A30" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="123"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="124">
+      <c r="C30" s="110"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="111">
         <f>SUM(F31:F35)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="114"/>
-      <c r="I30" s="124">
+      <c r="H30" s="102"/>
+      <c r="I30" s="111">
         <f>SUM(H31:H35)</f>
         <v>0</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="125"/>
-      <c r="N30" s="125"/>
-      <c r="O30" s="125"/>
-      <c r="P30" s="125"/>
-      <c r="Q30" s="125"/>
-      <c r="R30" s="126"/>
-      <c r="S30" s="127">
+      <c r="M30" s="112"/>
+      <c r="N30" s="112"/>
+      <c r="O30" s="112"/>
+      <c r="P30" s="112"/>
+      <c r="Q30" s="112"/>
+      <c r="R30" s="112"/>
+      <c r="S30" s="113">
         <f>SUM(M30:R30)</f>
         <v>0</v>
       </c>
@@ -2762,25 +2729,25 @@
       <c r="AH30" s="5"/>
     </row>
     <row r="31" ht="15.0" customHeight="1">
-      <c r="A31" s="122"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="129"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="130"/>
+      <c r="A31" s="109"/>
+      <c r="B31" s="114"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="116"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="131"/>
-      <c r="N31" s="131"/>
-      <c r="O31" s="131"/>
-      <c r="P31" s="131"/>
-      <c r="Q31" s="131"/>
-      <c r="R31" s="132"/>
-      <c r="S31" s="133"/>
+      <c r="M31" s="117"/>
+      <c r="N31" s="117"/>
+      <c r="O31" s="117"/>
+      <c r="P31" s="117"/>
+      <c r="Q31" s="117"/>
+      <c r="R31" s="117"/>
+      <c r="S31" s="118"/>
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
@@ -2798,25 +2765,25 @@
       <c r="AH31" s="4"/>
     </row>
     <row r="32" ht="15.0" customHeight="1">
-      <c r="A32" s="122"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="129"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="130"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="130"/>
+      <c r="A32" s="109"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="116"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="131"/>
-      <c r="N32" s="131"/>
-      <c r="O32" s="131"/>
-      <c r="P32" s="131"/>
-      <c r="Q32" s="131"/>
-      <c r="R32" s="132"/>
-      <c r="S32" s="133"/>
+      <c r="M32" s="117"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="117"/>
+      <c r="P32" s="117"/>
+      <c r="Q32" s="117"/>
+      <c r="R32" s="117"/>
+      <c r="S32" s="118"/>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
@@ -2834,25 +2801,25 @@
       <c r="AH32" s="4"/>
     </row>
     <row r="33" ht="15.0" customHeight="1">
-      <c r="A33" s="122"/>
-      <c r="B33" s="128"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="130"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="130"/>
+      <c r="A33" s="109"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="116"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="116"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="131"/>
-      <c r="N33" s="131"/>
-      <c r="O33" s="131"/>
-      <c r="P33" s="131"/>
-      <c r="Q33" s="131"/>
-      <c r="R33" s="132"/>
-      <c r="S33" s="133"/>
+      <c r="M33" s="117"/>
+      <c r="N33" s="117"/>
+      <c r="O33" s="117"/>
+      <c r="P33" s="117"/>
+      <c r="Q33" s="117"/>
+      <c r="R33" s="117"/>
+      <c r="S33" s="118"/>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
@@ -2870,25 +2837,25 @@
       <c r="AH33" s="4"/>
     </row>
     <row r="34" ht="15.0" customHeight="1">
-      <c r="A34" s="122"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="129"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="130"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="130"/>
+      <c r="A34" s="109"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="116"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="131"/>
-      <c r="N34" s="131"/>
-      <c r="O34" s="131"/>
-      <c r="P34" s="131"/>
-      <c r="Q34" s="131"/>
-      <c r="R34" s="132"/>
-      <c r="S34" s="133"/>
+      <c r="M34" s="117"/>
+      <c r="N34" s="117"/>
+      <c r="O34" s="117"/>
+      <c r="P34" s="117"/>
+      <c r="Q34" s="117"/>
+      <c r="R34" s="117"/>
+      <c r="S34" s="118"/>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
@@ -2906,25 +2873,25 @@
       <c r="AH34" s="4"/>
     </row>
     <row r="35" ht="15.0" customHeight="1">
-      <c r="A35" s="122"/>
-      <c r="B35" s="134"/>
-      <c r="C35" s="135"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="137"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="138"/>
-      <c r="I35" s="139"/>
+      <c r="A35" s="109"/>
+      <c r="B35" s="119"/>
+      <c r="C35" s="120"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="122"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="123"/>
+      <c r="I35" s="124"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="140"/>
-      <c r="N35" s="140"/>
-      <c r="O35" s="140"/>
-      <c r="P35" s="140"/>
-      <c r="Q35" s="140"/>
-      <c r="R35" s="141"/>
-      <c r="S35" s="142"/>
+      <c r="M35" s="125"/>
+      <c r="N35" s="125"/>
+      <c r="O35" s="125"/>
+      <c r="P35" s="125"/>
+      <c r="Q35" s="125"/>
+      <c r="R35" s="125"/>
+      <c r="S35" s="126"/>
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
@@ -2942,33 +2909,33 @@
       <c r="AH35" s="4"/>
     </row>
     <row r="36" ht="15.0" customHeight="1">
-      <c r="A36" s="122"/>
-      <c r="B36" s="36" t="s">
+      <c r="A36" s="109"/>
+      <c r="B36" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="123"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="114"/>
-      <c r="G36" s="124">
+      <c r="C36" s="110"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="102"/>
+      <c r="G36" s="111">
         <f>SUM(F37:F41)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="114"/>
-      <c r="I36" s="124">
+      <c r="H36" s="102"/>
+      <c r="I36" s="111">
         <f>SUM(H37:H41)</f>
         <v>0</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="125"/>
-      <c r="N36" s="125"/>
-      <c r="O36" s="125"/>
-      <c r="P36" s="125"/>
-      <c r="Q36" s="125"/>
-      <c r="R36" s="126"/>
-      <c r="S36" s="127">
+      <c r="M36" s="112"/>
+      <c r="N36" s="112"/>
+      <c r="O36" s="112"/>
+      <c r="P36" s="112"/>
+      <c r="Q36" s="112"/>
+      <c r="R36" s="112"/>
+      <c r="S36" s="113">
         <f>SUM(M36:R36)</f>
         <v>0</v>
       </c>
@@ -2989,25 +2956,25 @@
       <c r="AH36" s="4"/>
     </row>
     <row r="37" ht="15.0" customHeight="1">
-      <c r="A37" s="122"/>
-      <c r="B37" s="128"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="129"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="130"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="130"/>
+      <c r="A37" s="109"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="115"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="116"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="116"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="131"/>
-      <c r="N37" s="131"/>
-      <c r="O37" s="131"/>
-      <c r="P37" s="131"/>
-      <c r="Q37" s="131"/>
-      <c r="R37" s="132"/>
-      <c r="S37" s="133"/>
+      <c r="M37" s="117"/>
+      <c r="N37" s="117"/>
+      <c r="O37" s="117"/>
+      <c r="P37" s="117"/>
+      <c r="Q37" s="117"/>
+      <c r="R37" s="117"/>
+      <c r="S37" s="118"/>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
@@ -3025,25 +2992,25 @@
       <c r="AH37" s="4"/>
     </row>
     <row r="38" ht="15.0" customHeight="1">
-      <c r="A38" s="122"/>
-      <c r="B38" s="128"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="129"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="130"/>
+      <c r="A38" s="109"/>
+      <c r="B38" s="114"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="116"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="116"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" s="131"/>
-      <c r="N38" s="131"/>
-      <c r="O38" s="131"/>
-      <c r="P38" s="131"/>
-      <c r="Q38" s="131"/>
-      <c r="R38" s="132"/>
-      <c r="S38" s="133"/>
+      <c r="M38" s="117"/>
+      <c r="N38" s="117"/>
+      <c r="O38" s="117"/>
+      <c r="P38" s="117"/>
+      <c r="Q38" s="117"/>
+      <c r="R38" s="117"/>
+      <c r="S38" s="118"/>
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
@@ -3061,25 +3028,25 @@
       <c r="AH38" s="4"/>
     </row>
     <row r="39" ht="29.25" customHeight="1">
-      <c r="A39" s="122"/>
-      <c r="B39" s="128"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="129"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="130"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="130"/>
+      <c r="A39" s="109"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="116"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="116"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="131"/>
-      <c r="N39" s="131"/>
-      <c r="O39" s="131"/>
-      <c r="P39" s="131"/>
-      <c r="Q39" s="131"/>
-      <c r="R39" s="132"/>
-      <c r="S39" s="133"/>
+      <c r="M39" s="117"/>
+      <c r="N39" s="117"/>
+      <c r="O39" s="117"/>
+      <c r="P39" s="117"/>
+      <c r="Q39" s="117"/>
+      <c r="R39" s="117"/>
+      <c r="S39" s="118"/>
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
@@ -3097,25 +3064,25 @@
       <c r="AH39" s="4"/>
     </row>
     <row r="40" ht="15.0" customHeight="1">
-      <c r="A40" s="122"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="129"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="49"/>
-      <c r="I40" s="130"/>
+      <c r="A40" s="109"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="116"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="116"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="131"/>
-      <c r="N40" s="131"/>
-      <c r="O40" s="131"/>
-      <c r="P40" s="131"/>
-      <c r="Q40" s="131"/>
-      <c r="R40" s="132"/>
-      <c r="S40" s="133"/>
+      <c r="M40" s="117"/>
+      <c r="N40" s="117"/>
+      <c r="O40" s="117"/>
+      <c r="P40" s="117"/>
+      <c r="Q40" s="117"/>
+      <c r="R40" s="117"/>
+      <c r="S40" s="118"/>
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
@@ -3133,25 +3100,25 @@
       <c r="AH40" s="4"/>
     </row>
     <row r="41" ht="15.0" customHeight="1">
-      <c r="A41" s="122"/>
-      <c r="B41" s="134"/>
-      <c r="C41" s="135"/>
-      <c r="D41" s="136"/>
-      <c r="E41" s="137"/>
-      <c r="F41" s="138"/>
-      <c r="G41" s="139"/>
-      <c r="H41" s="138"/>
-      <c r="I41" s="139"/>
+      <c r="A41" s="109"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="121"/>
+      <c r="E41" s="122"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="124"/>
+      <c r="H41" s="123"/>
+      <c r="I41" s="124"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="140"/>
-      <c r="N41" s="140"/>
-      <c r="O41" s="140"/>
-      <c r="P41" s="140"/>
-      <c r="Q41" s="140"/>
-      <c r="R41" s="141"/>
-      <c r="S41" s="142"/>
+      <c r="M41" s="125"/>
+      <c r="N41" s="125"/>
+      <c r="O41" s="125"/>
+      <c r="P41" s="125"/>
+      <c r="Q41" s="125"/>
+      <c r="R41" s="125"/>
+      <c r="S41" s="126"/>
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
@@ -3169,33 +3136,33 @@
       <c r="AH41" s="4"/>
     </row>
     <row r="42" ht="15.0" customHeight="1">
-      <c r="A42" s="122"/>
-      <c r="B42" s="36" t="s">
+      <c r="A42" s="109"/>
+      <c r="B42" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="123"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="114"/>
-      <c r="G42" s="124">
+      <c r="C42" s="110"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="102"/>
+      <c r="G42" s="111">
         <f>SUM(F43:F45)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="114"/>
-      <c r="I42" s="124">
+      <c r="H42" s="102"/>
+      <c r="I42" s="111">
         <f>SUM(H43:H45)</f>
         <v>0</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="125"/>
-      <c r="N42" s="125"/>
-      <c r="O42" s="125"/>
-      <c r="P42" s="125"/>
-      <c r="Q42" s="125"/>
-      <c r="R42" s="126"/>
-      <c r="S42" s="127">
+      <c r="M42" s="112"/>
+      <c r="N42" s="112"/>
+      <c r="O42" s="112"/>
+      <c r="P42" s="112"/>
+      <c r="Q42" s="112"/>
+      <c r="R42" s="112"/>
+      <c r="S42" s="113">
         <f>SUM(M42:R42)</f>
         <v>0</v>
       </c>
@@ -3216,25 +3183,25 @@
       <c r="AH42" s="4"/>
     </row>
     <row r="43" ht="15.0" customHeight="1">
-      <c r="A43" s="122"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="129"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="130"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="130"/>
+      <c r="A43" s="109"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="115"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="116"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="116"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="131"/>
-      <c r="N43" s="131"/>
-      <c r="O43" s="131"/>
-      <c r="P43" s="131"/>
-      <c r="Q43" s="131"/>
-      <c r="R43" s="132"/>
-      <c r="S43" s="133"/>
+      <c r="M43" s="117"/>
+      <c r="N43" s="117"/>
+      <c r="O43" s="117"/>
+      <c r="P43" s="117"/>
+      <c r="Q43" s="117"/>
+      <c r="R43" s="117"/>
+      <c r="S43" s="118"/>
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
@@ -3252,25 +3219,25 @@
       <c r="AH43" s="4"/>
     </row>
     <row r="44" ht="15.0" customHeight="1">
-      <c r="A44" s="122"/>
-      <c r="B44" s="128"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="143"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="130"/>
+      <c r="A44" s="109"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="116"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="116"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="131"/>
-      <c r="N44" s="131"/>
-      <c r="O44" s="131"/>
-      <c r="P44" s="131"/>
-      <c r="Q44" s="131"/>
-      <c r="R44" s="132"/>
-      <c r="S44" s="133"/>
+      <c r="M44" s="117"/>
+      <c r="N44" s="117"/>
+      <c r="O44" s="117"/>
+      <c r="P44" s="117"/>
+      <c r="Q44" s="117"/>
+      <c r="R44" s="117"/>
+      <c r="S44" s="118"/>
       <c r="T44" s="4"/>
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
@@ -3288,25 +3255,25 @@
       <c r="AH44" s="4"/>
     </row>
     <row r="45" ht="15.0" customHeight="1">
-      <c r="A45" s="122"/>
-      <c r="B45" s="134"/>
-      <c r="C45" s="135"/>
-      <c r="D45" s="136"/>
-      <c r="E45" s="137"/>
-      <c r="F45" s="138"/>
-      <c r="G45" s="139"/>
-      <c r="H45" s="138"/>
-      <c r="I45" s="139"/>
+      <c r="A45" s="109"/>
+      <c r="B45" s="119"/>
+      <c r="C45" s="120"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="124"/>
+      <c r="H45" s="123"/>
+      <c r="I45" s="124"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="140"/>
-      <c r="N45" s="140"/>
-      <c r="O45" s="140"/>
-      <c r="P45" s="140"/>
-      <c r="Q45" s="140"/>
-      <c r="R45" s="141"/>
-      <c r="S45" s="142"/>
+      <c r="M45" s="125"/>
+      <c r="N45" s="125"/>
+      <c r="O45" s="125"/>
+      <c r="P45" s="125"/>
+      <c r="Q45" s="125"/>
+      <c r="R45" s="125"/>
+      <c r="S45" s="126"/>
       <c r="T45" s="4"/>
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
@@ -3324,35 +3291,35 @@
       <c r="AH45" s="4"/>
     </row>
     <row r="46" ht="15.0" customHeight="1">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="123"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="77"/>
-      <c r="G46" s="124">
+      <c r="C46" s="110"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="71"/>
+      <c r="G46" s="111">
         <f>SUM(F47:F50)</f>
         <v>0</v>
       </c>
-      <c r="H46" s="77"/>
-      <c r="I46" s="124">
+      <c r="H46" s="71"/>
+      <c r="I46" s="111">
         <f>SUM(H47:H50)</f>
         <v>0</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
-      <c r="M46" s="125"/>
-      <c r="N46" s="125"/>
-      <c r="O46" s="125"/>
-      <c r="P46" s="125"/>
-      <c r="Q46" s="125"/>
-      <c r="R46" s="126"/>
-      <c r="S46" s="127">
+      <c r="M46" s="112"/>
+      <c r="N46" s="112"/>
+      <c r="O46" s="112"/>
+      <c r="P46" s="112"/>
+      <c r="Q46" s="112"/>
+      <c r="R46" s="112"/>
+      <c r="S46" s="113">
         <f>SUM(M46:R46)</f>
         <v>0</v>
       </c>
@@ -3373,25 +3340,25 @@
       <c r="AH46" s="5"/>
     </row>
     <row r="47" ht="15.0" customHeight="1">
-      <c r="A47" s="144"/>
-      <c r="B47" s="145"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="146"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="147"/>
-      <c r="H47" s="65"/>
-      <c r="I47" s="148"/>
+      <c r="A47" s="128"/>
+      <c r="B47" s="129"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="130"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="131"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="132"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="149"/>
-      <c r="N47" s="149"/>
-      <c r="O47" s="149"/>
-      <c r="P47" s="149"/>
-      <c r="Q47" s="149"/>
-      <c r="R47" s="150"/>
-      <c r="S47" s="151"/>
+      <c r="M47" s="133"/>
+      <c r="N47" s="133"/>
+      <c r="O47" s="133"/>
+      <c r="P47" s="133"/>
+      <c r="Q47" s="133"/>
+      <c r="R47" s="133"/>
+      <c r="S47" s="134"/>
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
@@ -3409,25 +3376,25 @@
       <c r="AH47" s="4"/>
     </row>
     <row r="48" ht="15.0" customHeight="1">
-      <c r="A48" s="72"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="92"/>
-      <c r="D48" s="93"/>
-      <c r="E48" s="152"/>
-      <c r="F48" s="153"/>
-      <c r="G48" s="86"/>
-      <c r="H48" s="153"/>
-      <c r="I48" s="86"/>
+      <c r="A48" s="66"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="135"/>
+      <c r="F48" s="136"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="136"/>
+      <c r="I48" s="79"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="117"/>
-      <c r="N48" s="117"/>
-      <c r="O48" s="117"/>
-      <c r="P48" s="117"/>
-      <c r="Q48" s="117"/>
-      <c r="R48" s="119"/>
-      <c r="S48" s="121"/>
+      <c r="M48" s="107"/>
+      <c r="N48" s="107"/>
+      <c r="O48" s="107"/>
+      <c r="P48" s="107"/>
+      <c r="Q48" s="107"/>
+      <c r="R48" s="107"/>
+      <c r="S48" s="108"/>
       <c r="T48" s="4"/>
       <c r="U48" s="4"/>
       <c r="V48" s="4"/>
@@ -3445,25 +3412,25 @@
       <c r="AH48" s="4"/>
     </row>
     <row r="49" ht="15.0" customHeight="1">
-      <c r="A49" s="72"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="92"/>
-      <c r="D49" s="93"/>
-      <c r="E49" s="154"/>
-      <c r="F49" s="153"/>
-      <c r="G49" s="86"/>
-      <c r="H49" s="153"/>
-      <c r="I49" s="86"/>
+      <c r="A49" s="66"/>
+      <c r="B49" s="88"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="137"/>
+      <c r="F49" s="136"/>
+      <c r="G49" s="79"/>
+      <c r="H49" s="136"/>
+      <c r="I49" s="79"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="117"/>
-      <c r="N49" s="117"/>
-      <c r="O49" s="117"/>
-      <c r="P49" s="117"/>
-      <c r="Q49" s="117"/>
-      <c r="R49" s="119"/>
-      <c r="S49" s="121"/>
+      <c r="M49" s="107"/>
+      <c r="N49" s="107"/>
+      <c r="O49" s="107"/>
+      <c r="P49" s="107"/>
+      <c r="Q49" s="107"/>
+      <c r="R49" s="107"/>
+      <c r="S49" s="108"/>
       <c r="T49" s="4"/>
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
@@ -3481,25 +3448,25 @@
       <c r="AH49" s="4"/>
     </row>
     <row r="50" ht="15.0" customHeight="1">
-      <c r="A50" s="72"/>
-      <c r="B50" s="103"/>
-      <c r="C50" s="155"/>
-      <c r="D50" s="105"/>
-      <c r="E50" s="156"/>
-      <c r="F50" s="157"/>
-      <c r="G50" s="108"/>
-      <c r="H50" s="157"/>
-      <c r="I50" s="108"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="92"/>
+      <c r="C50" s="138"/>
+      <c r="D50" s="94"/>
+      <c r="E50" s="139"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="97"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="97"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="158"/>
-      <c r="N50" s="158"/>
-      <c r="O50" s="158"/>
-      <c r="P50" s="158"/>
-      <c r="Q50" s="158"/>
-      <c r="R50" s="159"/>
-      <c r="S50" s="160"/>
+      <c r="M50" s="141"/>
+      <c r="N50" s="141"/>
+      <c r="O50" s="141"/>
+      <c r="P50" s="141"/>
+      <c r="Q50" s="141"/>
+      <c r="R50" s="141"/>
+      <c r="S50" s="142"/>
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
@@ -3517,33 +3484,33 @@
       <c r="AH50" s="4"/>
     </row>
     <row r="51" ht="15.0" customHeight="1">
-      <c r="A51" s="72"/>
-      <c r="B51" s="36" t="s">
+      <c r="A51" s="66"/>
+      <c r="B51" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="123"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="76"/>
-      <c r="F51" s="114"/>
-      <c r="G51" s="124">
+      <c r="C51" s="110"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="102"/>
+      <c r="G51" s="111">
         <f>SUM(F52:F56)</f>
         <v>0</v>
       </c>
-      <c r="H51" s="114"/>
-      <c r="I51" s="124">
+      <c r="H51" s="102"/>
+      <c r="I51" s="111">
         <f>SUM(H52:H56)</f>
         <v>0</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="125"/>
-      <c r="N51" s="125"/>
-      <c r="O51" s="125"/>
-      <c r="P51" s="125"/>
-      <c r="Q51" s="125"/>
-      <c r="R51" s="126"/>
-      <c r="S51" s="127">
+      <c r="M51" s="112"/>
+      <c r="N51" s="112"/>
+      <c r="O51" s="112"/>
+      <c r="P51" s="112"/>
+      <c r="Q51" s="112"/>
+      <c r="R51" s="112"/>
+      <c r="S51" s="113">
         <f>SUM(M51:R51)</f>
         <v>0</v>
       </c>
@@ -3564,25 +3531,25 @@
       <c r="AH51" s="4"/>
     </row>
     <row r="52" ht="15.0" customHeight="1">
-      <c r="A52" s="72"/>
-      <c r="B52" s="99"/>
-      <c r="C52" s="92"/>
-      <c r="D52" s="93"/>
-      <c r="E52" s="154"/>
-      <c r="F52" s="153"/>
-      <c r="G52" s="86"/>
-      <c r="H52" s="153"/>
-      <c r="I52" s="86"/>
+      <c r="A52" s="66"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="86"/>
+      <c r="E52" s="137"/>
+      <c r="F52" s="136"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="136"/>
+      <c r="I52" s="79"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="117"/>
-      <c r="N52" s="117"/>
-      <c r="O52" s="117"/>
-      <c r="P52" s="117"/>
-      <c r="Q52" s="117"/>
-      <c r="R52" s="119"/>
-      <c r="S52" s="121"/>
+      <c r="M52" s="107"/>
+      <c r="N52" s="107"/>
+      <c r="O52" s="107"/>
+      <c r="P52" s="107"/>
+      <c r="Q52" s="107"/>
+      <c r="R52" s="107"/>
+      <c r="S52" s="108"/>
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
       <c r="V52" s="4"/>
@@ -3600,25 +3567,25 @@
       <c r="AH52" s="4"/>
     </row>
     <row r="53" ht="29.25" customHeight="1">
-      <c r="A53" s="72"/>
-      <c r="B53" s="99"/>
-      <c r="C53" s="92"/>
-      <c r="D53" s="93"/>
-      <c r="E53" s="154"/>
-      <c r="F53" s="153"/>
-      <c r="G53" s="86"/>
-      <c r="H53" s="153"/>
-      <c r="I53" s="86"/>
+      <c r="A53" s="66"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="137"/>
+      <c r="F53" s="136"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="136"/>
+      <c r="I53" s="79"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="117"/>
-      <c r="N53" s="117"/>
-      <c r="O53" s="117"/>
-      <c r="P53" s="117"/>
-      <c r="Q53" s="117"/>
-      <c r="R53" s="119"/>
-      <c r="S53" s="121"/>
+      <c r="M53" s="107"/>
+      <c r="N53" s="107"/>
+      <c r="O53" s="107"/>
+      <c r="P53" s="107"/>
+      <c r="Q53" s="107"/>
+      <c r="R53" s="107"/>
+      <c r="S53" s="108"/>
       <c r="T53" s="4"/>
       <c r="U53" s="4"/>
       <c r="V53" s="4"/>
@@ -3636,25 +3603,25 @@
       <c r="AH53" s="4"/>
     </row>
     <row r="54" ht="15.0" customHeight="1">
-      <c r="A54" s="72"/>
-      <c r="B54" s="99"/>
-      <c r="C54" s="92"/>
-      <c r="D54" s="93"/>
-      <c r="E54" s="154"/>
-      <c r="F54" s="153"/>
-      <c r="G54" s="86"/>
-      <c r="H54" s="153"/>
-      <c r="I54" s="86"/>
+      <c r="A54" s="66"/>
+      <c r="B54" s="88"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="86"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="136"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="136"/>
+      <c r="I54" s="79"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="117"/>
-      <c r="N54" s="117"/>
-      <c r="O54" s="117"/>
-      <c r="P54" s="117"/>
-      <c r="Q54" s="117"/>
-      <c r="R54" s="119"/>
-      <c r="S54" s="121"/>
+      <c r="M54" s="107"/>
+      <c r="N54" s="107"/>
+      <c r="O54" s="107"/>
+      <c r="P54" s="107"/>
+      <c r="Q54" s="107"/>
+      <c r="R54" s="107"/>
+      <c r="S54" s="108"/>
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
       <c r="V54" s="4"/>
@@ -3672,25 +3639,25 @@
       <c r="AH54" s="4"/>
     </row>
     <row r="55" ht="15.0" customHeight="1">
-      <c r="A55" s="72"/>
-      <c r="B55" s="99"/>
-      <c r="C55" s="92"/>
-      <c r="D55" s="93"/>
-      <c r="E55" s="154"/>
-      <c r="F55" s="153"/>
-      <c r="G55" s="86"/>
-      <c r="H55" s="153"/>
-      <c r="I55" s="86"/>
+      <c r="A55" s="66"/>
+      <c r="B55" s="88"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="86"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="136"/>
+      <c r="G55" s="79"/>
+      <c r="H55" s="136"/>
+      <c r="I55" s="79"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="117"/>
-      <c r="N55" s="117"/>
-      <c r="O55" s="117"/>
-      <c r="P55" s="117"/>
-      <c r="Q55" s="117"/>
-      <c r="R55" s="119"/>
-      <c r="S55" s="121"/>
+      <c r="M55" s="107"/>
+      <c r="N55" s="107"/>
+      <c r="O55" s="107"/>
+      <c r="P55" s="107"/>
+      <c r="Q55" s="107"/>
+      <c r="R55" s="107"/>
+      <c r="S55" s="108"/>
       <c r="T55" s="4"/>
       <c r="U55" s="4"/>
       <c r="V55" s="4"/>
@@ -3708,25 +3675,25 @@
       <c r="AH55" s="4"/>
     </row>
     <row r="56" ht="15.0" customHeight="1">
-      <c r="A56" s="72"/>
-      <c r="B56" s="103"/>
-      <c r="C56" s="155"/>
-      <c r="D56" s="105"/>
-      <c r="E56" s="156"/>
-      <c r="F56" s="157"/>
-      <c r="G56" s="108"/>
-      <c r="H56" s="157"/>
-      <c r="I56" s="108"/>
+      <c r="A56" s="66"/>
+      <c r="B56" s="92"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="94"/>
+      <c r="E56" s="139"/>
+      <c r="F56" s="140"/>
+      <c r="G56" s="97"/>
+      <c r="H56" s="140"/>
+      <c r="I56" s="97"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="158"/>
-      <c r="N56" s="158"/>
-      <c r="O56" s="158"/>
-      <c r="P56" s="158"/>
-      <c r="Q56" s="158"/>
-      <c r="R56" s="159"/>
-      <c r="S56" s="160"/>
+      <c r="M56" s="141"/>
+      <c r="N56" s="141"/>
+      <c r="O56" s="141"/>
+      <c r="P56" s="141"/>
+      <c r="Q56" s="141"/>
+      <c r="R56" s="141"/>
+      <c r="S56" s="142"/>
       <c r="T56" s="4"/>
       <c r="U56" s="4"/>
       <c r="V56" s="4"/>
@@ -3744,33 +3711,33 @@
       <c r="AH56" s="4"/>
     </row>
     <row r="57" ht="15.0" customHeight="1">
-      <c r="A57" s="72"/>
-      <c r="B57" s="161" t="s">
+      <c r="A57" s="66"/>
+      <c r="B57" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="C57" s="162"/>
-      <c r="D57" s="163"/>
-      <c r="E57" s="164"/>
-      <c r="F57" s="165"/>
-      <c r="G57" s="166">
+      <c r="C57" s="144"/>
+      <c r="D57" s="145"/>
+      <c r="E57" s="146"/>
+      <c r="F57" s="147"/>
+      <c r="G57" s="148">
         <f>SUM(F58:F59)</f>
         <v>0</v>
       </c>
-      <c r="H57" s="165"/>
-      <c r="I57" s="166">
+      <c r="H57" s="147"/>
+      <c r="I57" s="148">
         <f>SUM(H58:H59)</f>
         <v>0</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="167"/>
-      <c r="N57" s="167"/>
-      <c r="O57" s="167"/>
-      <c r="P57" s="167"/>
-      <c r="Q57" s="167"/>
-      <c r="R57" s="168"/>
-      <c r="S57" s="169">
+      <c r="M57" s="149"/>
+      <c r="N57" s="149"/>
+      <c r="O57" s="149"/>
+      <c r="P57" s="149"/>
+      <c r="Q57" s="149"/>
+      <c r="R57" s="149"/>
+      <c r="S57" s="150">
         <f>SUM(M57:R57)</f>
         <v>0</v>
       </c>
@@ -3791,25 +3758,25 @@
       <c r="AH57" s="4"/>
     </row>
     <row r="58" ht="15.0" customHeight="1">
-      <c r="A58" s="144"/>
-      <c r="B58" s="145"/>
-      <c r="C58" s="62"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="64"/>
-      <c r="F58" s="170"/>
-      <c r="G58" s="147"/>
-      <c r="H58" s="170"/>
-      <c r="I58" s="148"/>
+      <c r="A58" s="128"/>
+      <c r="B58" s="129"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="60"/>
+      <c r="F58" s="151"/>
+      <c r="G58" s="131"/>
+      <c r="H58" s="151"/>
+      <c r="I58" s="132"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="149"/>
-      <c r="N58" s="149"/>
-      <c r="O58" s="149"/>
-      <c r="P58" s="149"/>
-      <c r="Q58" s="149"/>
-      <c r="R58" s="150"/>
-      <c r="S58" s="151"/>
+      <c r="M58" s="133"/>
+      <c r="N58" s="133"/>
+      <c r="O58" s="133"/>
+      <c r="P58" s="133"/>
+      <c r="Q58" s="133"/>
+      <c r="R58" s="133"/>
+      <c r="S58" s="134"/>
       <c r="T58" s="4"/>
       <c r="U58" s="4"/>
       <c r="V58" s="4"/>
@@ -3827,25 +3794,25 @@
       <c r="AH58" s="4"/>
     </row>
     <row r="59" ht="15.0" customHeight="1">
-      <c r="A59" s="171"/>
-      <c r="B59" s="103"/>
-      <c r="C59" s="155"/>
-      <c r="D59" s="105"/>
-      <c r="E59" s="172"/>
-      <c r="F59" s="157"/>
-      <c r="G59" s="108"/>
-      <c r="H59" s="157"/>
-      <c r="I59" s="108"/>
+      <c r="A59" s="152"/>
+      <c r="B59" s="92"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="153"/>
+      <c r="F59" s="140"/>
+      <c r="G59" s="97"/>
+      <c r="H59" s="140"/>
+      <c r="I59" s="97"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="158"/>
-      <c r="N59" s="158"/>
-      <c r="O59" s="158"/>
-      <c r="P59" s="158"/>
-      <c r="Q59" s="158"/>
-      <c r="R59" s="159"/>
-      <c r="S59" s="158"/>
+      <c r="M59" s="141"/>
+      <c r="N59" s="141"/>
+      <c r="O59" s="141"/>
+      <c r="P59" s="141"/>
+      <c r="Q59" s="141"/>
+      <c r="R59" s="141"/>
+      <c r="S59" s="141"/>
       <c r="T59" s="4"/>
       <c r="U59" s="4"/>
       <c r="V59" s="4"/>
@@ -3863,75 +3830,75 @@
       <c r="AH59" s="4"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="173" t="s">
+      <c r="A60" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="173"/>
-      <c r="C60" s="174"/>
-      <c r="D60" s="174"/>
-      <c r="E60" s="175"/>
-      <c r="F60" s="176">
+      <c r="B60" s="154"/>
+      <c r="C60" s="155"/>
+      <c r="D60" s="155"/>
+      <c r="E60" s="156"/>
+      <c r="F60" s="157">
         <f t="shared" ref="F60:G60" si="5">SUM(F5:F59)</f>
         <v>62</v>
       </c>
-      <c r="G60" s="177">
+      <c r="G60" s="158">
         <f t="shared" si="5"/>
         <v>62</v>
       </c>
-      <c r="H60" s="178">
+      <c r="H60" s="159">
         <f>SUM(M60:R60)</f>
-        <v>45</v>
+        <v>71.5</v>
       </c>
-      <c r="I60" s="177">
+      <c r="I60" s="158">
         <f>SUM(I5:I59)</f>
         <v>62</v>
       </c>
-      <c r="J60" s="179"/>
-      <c r="K60" s="179"/>
-      <c r="L60" s="179"/>
-      <c r="M60" s="178">
+      <c r="J60" s="160"/>
+      <c r="K60" s="160"/>
+      <c r="L60" s="160"/>
+      <c r="M60" s="159">
         <f t="shared" ref="M60:O60" si="6">SUM(M5:M59)</f>
-        <v>5.5</v>
+        <v>15.5</v>
       </c>
-      <c r="N60" s="178">
+      <c r="N60" s="159">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="O60" s="178">
+      <c r="O60" s="159">
         <f t="shared" si="6"/>
         <v>19.5</v>
       </c>
-      <c r="P60" s="178"/>
-      <c r="Q60" s="178"/>
-      <c r="R60" s="178">
+      <c r="P60" s="159"/>
+      <c r="Q60" s="159"/>
+      <c r="R60" s="159">
         <f>SUM(R5:R59)</f>
-        <v>0</v>
+        <v>16.5</v>
       </c>
-      <c r="S60" s="178">
+      <c r="S60" s="159">
         <f>SUM(M60:R60)</f>
-        <v>45</v>
+        <v>71.5</v>
       </c>
-      <c r="T60" s="179"/>
-      <c r="U60" s="179"/>
-      <c r="V60" s="179"/>
-      <c r="W60" s="179"/>
-      <c r="X60" s="179"/>
-      <c r="Y60" s="179"/>
-      <c r="Z60" s="179"/>
-      <c r="AA60" s="179"/>
-      <c r="AB60" s="179"/>
-      <c r="AC60" s="179"/>
-      <c r="AD60" s="179"/>
-      <c r="AE60" s="179"/>
-      <c r="AF60" s="179"/>
-      <c r="AG60" s="179"/>
-      <c r="AH60" s="179"/>
+      <c r="T60" s="160"/>
+      <c r="U60" s="160"/>
+      <c r="V60" s="160"/>
+      <c r="W60" s="160"/>
+      <c r="X60" s="160"/>
+      <c r="Y60" s="160"/>
+      <c r="Z60" s="160"/>
+      <c r="AA60" s="160"/>
+      <c r="AB60" s="160"/>
+      <c r="AC60" s="160"/>
+      <c r="AD60" s="160"/>
+      <c r="AE60" s="160"/>
+      <c r="AF60" s="160"/>
+      <c r="AG60" s="160"/>
+      <c r="AH60" s="160"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="180"/>
+      <c r="D61" s="161"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
@@ -3967,7 +3934,7 @@
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="180"/>
+      <c r="D62" s="161"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
@@ -4003,7 +3970,7 @@
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="180"/>
+      <c r="D63" s="161"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>

</xml_diff>